<commit_message>
add react + express
</commit_message>
<xml_diff>
--- a/data/transaction.xlsx
+++ b/data/transaction.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darrenmuliawan/Desktop/Projects/ember/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0665554-07BC-9741-89A6-DBD1CFD28CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B7F7F5-F845-0341-BA44-38495432DBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="500" windowWidth="22060" windowHeight="17440" xr2:uid="{57C7BA3C-F476-034B-B6FD-E16C331F6349}"/>
+    <workbookView xWindow="900" yWindow="500" windowWidth="28300" windowHeight="17440" xr2:uid="{57C7BA3C-F476-034B-B6FD-E16C331F6349}"/>
   </bookViews>
   <sheets>
     <sheet name="transaction" sheetId="1" r:id="rId1"/>
     <sheet name="deposit" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>date</t>
   </si>
@@ -140,6 +140,24 @@
   </si>
   <si>
     <t>Genworth Fincl</t>
+  </si>
+  <si>
+    <t>SELL</t>
+  </si>
+  <si>
+    <t>network_fee</t>
+  </si>
+  <si>
+    <t>network_fee_transfer_to_wallet</t>
+  </si>
+  <si>
+    <t>network_fee_pct</t>
+  </si>
+  <si>
+    <t>wallet_received</t>
+  </si>
+  <si>
+    <t>network_fee_transfer_to_wallet_pct</t>
   </si>
 </sst>
 </file>
@@ -147,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -180,7 +198,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15D7115-ED5D-C845-803B-AD43ED624E04}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,9 +527,14 @@
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+    <col min="11" max="11" width="32.33203125" customWidth="1"/>
+    <col min="12" max="12" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +556,23 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44342</v>
       </c>
@@ -554,11 +592,28 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <f>E2*F2</f>
+        <f t="shared" ref="G2:G18" si="0">E2*F2</f>
         <v>5400</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I16" si="1">(H2/F2)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="e">
+        <f t="shared" ref="L2:L16" si="2">(K2/J2)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44342</v>
       </c>
@@ -578,11 +633,28 @@
         <v>75</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G11" si="0">E3*F3</f>
+        <f t="shared" si="0"/>
         <v>3052.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44342</v>
       </c>
@@ -605,8 +677,25 @@
         <f t="shared" si="0"/>
         <v>1254.3000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44342</v>
       </c>
@@ -629,8 +718,25 @@
         <f t="shared" si="0"/>
         <v>2018.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44342</v>
       </c>
@@ -653,8 +759,25 @@
         <f t="shared" si="0"/>
         <v>873.09798499999988</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44342</v>
       </c>
@@ -677,8 +800,25 @@
         <f t="shared" si="0"/>
         <v>812.18</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44342</v>
       </c>
@@ -701,8 +841,25 @@
         <f t="shared" si="0"/>
         <v>754.96386000000007</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44342</v>
       </c>
@@ -725,8 +882,25 @@
         <f t="shared" si="0"/>
         <v>603.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44342</v>
       </c>
@@ -749,8 +923,25 @@
         <f t="shared" si="0"/>
         <v>15.22</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44342</v>
       </c>
@@ -772,6 +963,313 @@
       <c r="G11">
         <f t="shared" si="0"/>
         <v>6.26</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>1.5422400000000001</v>
+      </c>
+      <c r="F12">
+        <v>161</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>248.30064000000002</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>44345</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>1.365</v>
+      </c>
+      <c r="F13">
+        <v>153.9</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>210.0735</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>44345</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>1.4</v>
+      </c>
+      <c r="F14">
+        <v>178.2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>249.47999999999996</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <v>111</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>28.5</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>142.5</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>44353</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>36056.870000000003</v>
+      </c>
+      <c r="F17">
+        <v>6.9095399999999996E-3</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>249.13638553980002</v>
+      </c>
+      <c r="H17">
+        <f>F17-0.00689577</f>
+        <v>1.3769999999999755E-5</v>
+      </c>
+      <c r="I17">
+        <f>(H17/F17)*100</f>
+        <v>0.19928967774989009</v>
+      </c>
+      <c r="J17">
+        <v>6.8957699999999999E-3</v>
+      </c>
+      <c r="K17">
+        <f>F17-J17</f>
+        <v>1.3769999999999755E-5</v>
+      </c>
+      <c r="L17">
+        <f>(K17/J17)*100</f>
+        <v>0.19968763459337763</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44353</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>36147.65</v>
+      </c>
+      <c r="F18">
+        <v>6.8898300000000004E-3</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>249.05116339950001</v>
+      </c>
+      <c r="H18">
+        <v>2.4070000000000002E-5</v>
+      </c>
+      <c r="I18">
+        <f>(H18/F18)*100</f>
+        <v>0.34935549933742926</v>
+      </c>
+      <c r="J18">
+        <v>6.8790500000000003E-3</v>
+      </c>
+      <c r="K18">
+        <f>F18-J18</f>
+        <v>1.0780000000000164E-5</v>
+      </c>
+      <c r="L18">
+        <f>(K18/J18)*100</f>
+        <v>0.15670768492742695</v>
       </c>
     </row>
   </sheetData>
@@ -781,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9A5BB5-F6AD-7248-B463-2EA501F1B629}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,6 +1345,62 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44345</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44353</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>